<commit_message>
update kabupaten bandung data
</commit_message>
<xml_diff>
--- a/Dataset/kecamatan_kabupaten_bandung.xlsx
+++ b/Dataset/kecamatan_kabupaten_bandung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Colab Notebooks\Pacmann AI\Statistics\5-Sampling\Project\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C83A7-1414-40AF-AE6F-69AA8E3F10BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2554EA-3FF6-43D5-BA29-F0324FBB890B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA512314-67D6-4886-AC41-3F023F95669E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{EA512314-67D6-4886-AC41-3F023F95669E}"/>
   </bookViews>
   <sheets>
     <sheet name="kecamatan_kab_bandung" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="230">
   <si>
     <t>Kecamatan</t>
   </si>
@@ -556,9 +556,6 @@
     <t>Sukamenak</t>
   </si>
   <si>
-    <t>DYEUHKOLOT</t>
-  </si>
-  <si>
     <t>Citeureup</t>
   </si>
   <si>
@@ -664,18 +661,6 @@
     <t>Laju Pertumbuhan (2020-2021)</t>
   </si>
   <si>
-    <t>ΚΑΤΑΡΑΝG</t>
-  </si>
-  <si>
-    <t>DAYEUΗΚOLOΤ</t>
-  </si>
-  <si>
-    <t>CILEUΝΥΙ</t>
-  </si>
-  <si>
-    <t>CΙΜΕΝΥΑΝ</t>
-  </si>
-  <si>
     <t>Persentase Penduduk (2020)</t>
   </si>
   <si>
@@ -686,9 +671,6 @@
   </si>
   <si>
     <t>Kepadatan Penduduk (2021)</t>
-  </si>
-  <si>
-    <t>MARGAASlH</t>
   </si>
   <si>
     <t>DAYEUHKOLOT</t>
@@ -1169,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEF4BC-707C-45E2-9F83-C7A793232829}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1963,8 +1945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1576BF-FD72-4773-8929-C5AD0E0EA42B}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,18 +1961,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C2" s="1">
         <v>48.47</v>
@@ -1998,10 +1980,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="C3" s="1">
         <v>148.37</v>
@@ -2009,7 +1991,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>131</v>
@@ -2020,10 +2002,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="C5" s="1">
         <v>55</v>
@@ -2031,7 +2013,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>123</v>
@@ -2042,10 +2024,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C7" s="1">
         <v>152.07</v>
@@ -2053,10 +2035,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C8" s="1">
         <v>91.94</v>
@@ -2064,10 +2046,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="C9" s="1">
         <v>54.57</v>
@@ -2075,10 +2057,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="C10" s="1">
         <v>51.03</v>
@@ -2086,7 +2068,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>41</v>
@@ -2097,10 +2079,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="C12" s="1">
         <v>35.99</v>
@@ -2108,10 +2090,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C13" s="1">
         <v>49.3</v>
@@ -2119,10 +2101,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="C14" s="1">
         <v>45.25</v>
@@ -2273,10 +2255,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C28" s="1">
         <v>11.03</v>
@@ -2284,7 +2266,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
@@ -2295,7 +2277,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>50</v>
@@ -2306,10 +2288,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="C31" s="1">
         <v>30.12</v>
@@ -2317,7 +2299,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>59</v>
@@ -2328,6 +2310,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2335,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE7FA8C-25BC-416E-9726-30FC685026AD}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A32" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,21 +2334,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="1">
         <v>86445</v>
@@ -2382,7 +2365,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1">
         <v>51096</v>
@@ -2399,7 +2382,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1">
         <v>91191</v>
@@ -2416,7 +2399,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1">
         <v>86075</v>
@@ -2433,7 +2416,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1">
         <v>154286</v>
@@ -2450,7 +2433,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1">
         <v>71255</v>
@@ -2467,7 +2450,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1">
         <v>115066</v>
@@ -2484,7 +2467,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="1">
         <v>87020</v>
@@ -2501,7 +2484,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1">
         <v>136202</v>
@@ -2518,7 +2501,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="1">
         <v>96710</v>
@@ -2535,7 +2518,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" s="1">
         <v>122162</v>
@@ -2552,7 +2535,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" s="1">
         <v>58408</v>
@@ -2569,7 +2552,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1">
         <v>185499</v>
@@ -2722,7 +2705,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>206</v>
+        <v>162</v>
       </c>
       <c r="B23" s="1">
         <v>130417</v>
@@ -2807,7 +2790,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B28" s="1">
         <v>107186</v>
@@ -2824,7 +2807,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="1">
         <v>112671</v>
@@ -2841,7 +2824,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="B30" s="1">
         <v>186543</v>
@@ -2858,7 +2841,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="1">
         <v>56018</v>
@@ -2875,7 +2858,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="B32" s="1">
         <v>114567</v>
@@ -2899,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E337745-D816-4023-828E-A040075FCD59}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A32" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,21 +2898,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="1">
         <v>2.39</v>
@@ -2946,7 +2929,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1">
         <v>1.41</v>
@@ -2963,7 +2946,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1">
         <v>2.52</v>
@@ -2980,7 +2963,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1">
         <v>2.38</v>
@@ -2997,7 +2980,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1">
         <v>4.26</v>
@@ -3014,7 +2997,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1">
         <v>1.97</v>
@@ -3031,7 +3014,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1">
         <v>3.18</v>
@@ -3048,7 +3031,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="1">
         <v>2.4</v>
@@ -3065,7 +3048,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1">
         <v>3.76</v>
@@ -3082,7 +3065,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="1">
         <v>2.67</v>
@@ -3099,7 +3082,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" s="1">
         <v>3.37</v>
@@ -3116,7 +3099,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" s="1">
         <v>1.61</v>
@@ -3133,7 +3116,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1">
         <v>5.12</v>
@@ -3286,7 +3269,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>206</v>
+        <v>162</v>
       </c>
       <c r="B23" s="1">
         <v>3.6</v>
@@ -3337,7 +3320,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="B26" s="1">
         <v>4.0999999999999996</v>
@@ -3371,7 +3354,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B28" s="1">
         <v>2.96</v>
@@ -3388,7 +3371,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="1">
         <v>3.11</v>
@@ -3405,7 +3388,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="1">
         <v>5.15</v>
@@ -3422,7 +3405,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="1">
         <v>1.55</v>
@@ -3439,7 +3422,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B32" s="1">
         <v>3.16</v>
@@ -3477,21 +3460,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B2" s="1">
         <v>161971</v>
@@ -3505,7 +3488,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B3" s="1">
         <v>157161</v>
@@ -3519,7 +3502,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B4" s="1">
         <v>171611</v>
@@ -3533,7 +3516,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B5" s="1">
         <v>166668</v>
@@ -3547,7 +3530,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B6" s="1">
         <v>158191</v>
@@ -3561,7 +3544,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1">
         <v>154199</v>
@@ -3575,7 +3558,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B8" s="1">
         <v>144649</v>
@@ -3589,7 +3572,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B9" s="1">
         <v>145686</v>
@@ -3603,7 +3586,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B10" s="1">
         <v>140981</v>
@@ -3617,7 +3600,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B11" s="1">
         <v>123727</v>
@@ -3631,7 +3614,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B12" s="1">
         <v>103251</v>
@@ -3645,7 +3628,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B13" s="1">
         <v>84559</v>
@@ -3659,7 +3642,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B14" s="1">
         <v>63372</v>
@@ -3673,7 +3656,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B15" s="1">
         <v>46177</v>
@@ -3687,7 +3670,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B16" s="1">
         <v>25649</v>
@@ -3701,7 +3684,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B17" s="1">
         <v>21157</v>

</xml_diff>